<commit_message>
obtenção de dados de empresas a partir das entidadse encontradas
</commit_message>
<xml_diff>
--- a/docs/lista_portais_transparencia.xlsx
+++ b/docs/lista_portais_transparencia.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samuel\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Monique\Documents\TCU\SecexSaude\CoviDATA\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046A1CD1-0809-41C8-A87C-888D699262CF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0591ECA-156C-4334-98F5-37092ED18AF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dados" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -765,22 +764,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="121.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="99.7109375" customWidth="1"/>
-    <col min="4" max="4" width="47.7109375" customWidth="1"/>
-    <col min="5" max="5" width="96.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="53.28515625" customWidth="1"/>
-    <col min="7" max="7" width="111.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="121.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="99.6640625" customWidth="1"/>
+    <col min="4" max="4" width="47.6640625" customWidth="1"/>
+    <col min="5" max="5" width="96.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="53.33203125" customWidth="1"/>
+    <col min="7" max="7" width="111.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -803,7 +802,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -826,7 +825,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -849,7 +848,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -872,7 +871,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -895,7 +894,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>51</v>
       </c>
@@ -918,7 +917,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>50</v>
       </c>
@@ -929,7 +928,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -952,7 +951,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -975,7 +974,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -998,7 +997,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>56</v>
       </c>
@@ -1021,7 +1020,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>55</v>
       </c>
@@ -1044,7 +1043,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -1067,7 +1066,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -1090,7 +1089,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -1113,7 +1112,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -1136,7 +1135,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -1159,7 +1158,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>52</v>
       </c>
@@ -1182,7 +1181,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -1205,7 +1204,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -1228,7 +1227,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -1251,7 +1250,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -1274,7 +1273,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>62</v>
       </c>
@@ -1297,7 +1296,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>61</v>
       </c>
@@ -1320,7 +1319,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -1343,7 +1342,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -1366,7 +1365,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>17</v>
       </c>
@@ -1389,7 +1388,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>18</v>
       </c>
@@ -1412,7 +1411,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>19</v>
       </c>
@@ -1435,7 +1434,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>59</v>
       </c>
@@ -1458,7 +1457,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>58</v>
       </c>
@@ -1481,7 +1480,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>20</v>
       </c>
@@ -1501,7 +1500,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>21</v>
       </c>

</xml_diff>